<commit_message>
i don't now what i change
</commit_message>
<xml_diff>
--- a/templates/note_for_change.xlsx
+++ b/templates/note_for_change.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Bảng\Ngày</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>slug field, password, slug for change information</t>
+  </si>
+  <si>
+    <t>banner_image</t>
+  </si>
+  <si>
+    <t>field for motobikes</t>
   </si>
 </sst>
 </file>
@@ -391,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:B16"/>
+  <dimension ref="A4:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,6 +502,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>